<commit_message>
ejercicio 1 cambio excel y rediseño de base de datos en case studio
</commit_message>
<xml_diff>
--- a/ejercicio 1 punto de venta Jorge Gutierrez/ejercicio1 punto de venta.xlsx
+++ b/ejercicio 1 punto de venta Jorge Gutierrez/ejercicio1 punto de venta.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Cliente" sheetId="1" r:id="rId1"/>
-    <sheet name="Encabezado" sheetId="5" r:id="rId2"/>
-    <sheet name="Detalle" sheetId="2" r:id="rId3"/>
-    <sheet name="Producto" sheetId="3" r:id="rId4"/>
-    <sheet name="Proveedor" sheetId="4" r:id="rId5"/>
+    <sheet name="Departamento" sheetId="6" r:id="rId1"/>
+    <sheet name="Municipio" sheetId="7" r:id="rId2"/>
+    <sheet name="Cliente" sheetId="1" r:id="rId3"/>
+    <sheet name="Encabezado_Compra" sheetId="5" r:id="rId4"/>
+    <sheet name="Detalle_Compra" sheetId="2" r:id="rId5"/>
+    <sheet name="Producto" sheetId="3" r:id="rId6"/>
+    <sheet name="Detalle_Venta" sheetId="9" r:id="rId7"/>
+    <sheet name="Encabezado_Venta" sheetId="8" r:id="rId8"/>
+    <sheet name="Proveedor" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>dpi_cliente</t>
   </si>
@@ -81,24 +85,6 @@
     <t>Lopez Urizar</t>
   </si>
   <si>
-    <t>zona 3 Quetzaltenango</t>
-  </si>
-  <si>
-    <t>zona 1 Zacapa</t>
-  </si>
-  <si>
-    <t>5ta avenida zona 1 Guatemala</t>
-  </si>
-  <si>
-    <t>colonia Molina Quetzaltenango</t>
-  </si>
-  <si>
-    <t>Salcaja Quetzaltenango</t>
-  </si>
-  <si>
-    <t>Zona 1 Sa Marcos</t>
-  </si>
-  <si>
     <t>codigo_producto</t>
   </si>
   <si>
@@ -108,9 +94,6 @@
     <t>nombre_producto</t>
   </si>
   <si>
-    <t>precio_producto</t>
-  </si>
-  <si>
     <t>existencia_producto</t>
   </si>
   <si>
@@ -147,27 +130,6 @@
     <t>Industrias totales S.A.</t>
   </si>
   <si>
-    <t>zona 3, Guatemala</t>
-  </si>
-  <si>
-    <t>Mixco, Guatemala</t>
-  </si>
-  <si>
-    <t>Chimatenango, Guatemala</t>
-  </si>
-  <si>
-    <t>zona 1 Peten</t>
-  </si>
-  <si>
-    <t>zona industrial, Guatemala</t>
-  </si>
-  <si>
-    <t>29 calle zona 3, Guatemala</t>
-  </si>
-  <si>
-    <t>Retalhuleu</t>
-  </si>
-  <si>
     <t>Margarina 50 gr.</t>
   </si>
   <si>
@@ -204,25 +166,145 @@
     <t>COD-GAS</t>
   </si>
   <si>
-    <t>codigo_encabezado</t>
-  </si>
-  <si>
-    <t>total_compra</t>
-  </si>
-  <si>
     <t>totalprod_compra</t>
   </si>
   <si>
-    <t>codigo_detalle</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">precio </t>
-  </si>
-  <si>
-    <t>subtotal</t>
+    <t>codigo_departamento</t>
+  </si>
+  <si>
+    <t>nombre_departamento</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Quetzaltenango</t>
+  </si>
+  <si>
+    <t>Totonicapan</t>
+  </si>
+  <si>
+    <t>Solola</t>
+  </si>
+  <si>
+    <t>San Marcos</t>
+  </si>
+  <si>
+    <t>Rethauleu</t>
+  </si>
+  <si>
+    <t>codigo_municipio</t>
+  </si>
+  <si>
+    <t>nombre_municipio</t>
+  </si>
+  <si>
+    <t>Mixco</t>
+  </si>
+  <si>
+    <t>Salcaja</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>San Juan La Laguna</t>
+  </si>
+  <si>
+    <t>Champerico</t>
+  </si>
+  <si>
+    <t>El Tumbador</t>
+  </si>
+  <si>
+    <t>Ayutla</t>
+  </si>
+  <si>
+    <t>Momostenango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zona 3 </t>
+  </si>
+  <si>
+    <t>zona 1</t>
+  </si>
+  <si>
+    <t>5ta avenida zona 1</t>
+  </si>
+  <si>
+    <t>Zona 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colonia Molina </t>
+  </si>
+  <si>
+    <t>codigo_encabezado_compra</t>
+  </si>
+  <si>
+    <t>totalQ_compra</t>
+  </si>
+  <si>
+    <t>codigo_detalle_compra</t>
+  </si>
+  <si>
+    <t>cantidad_compra</t>
+  </si>
+  <si>
+    <t>precio_compra</t>
+  </si>
+  <si>
+    <t>subtotal_compra</t>
+  </si>
+  <si>
+    <t>precio_venta_producto</t>
+  </si>
+  <si>
+    <t>precio_compra_producto</t>
+  </si>
+  <si>
+    <t>Chimaltenango</t>
+  </si>
+  <si>
+    <t>zona 3</t>
+  </si>
+  <si>
+    <t>zona 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zona 1 </t>
+  </si>
+  <si>
+    <t>zona industrial</t>
+  </si>
+  <si>
+    <t>29 calle zona 3</t>
+  </si>
+  <si>
+    <t>zona 2</t>
+  </si>
+  <si>
+    <t>codigo_encabezado_venta</t>
+  </si>
+  <si>
+    <t>fecha_venta</t>
+  </si>
+  <si>
+    <t>totalQ_venta</t>
+  </si>
+  <si>
+    <t>totalprod_venta</t>
+  </si>
+  <si>
+    <t>codigo_detalle_venta</t>
+  </si>
+  <si>
+    <t>cantidad_venta</t>
+  </si>
+  <si>
+    <t>precio_venta</t>
+  </si>
+  <si>
+    <t>subtotal_venta</t>
   </si>
 </sst>
 </file>
@@ -315,7 +397,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -347,6 +429,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -630,137 +719,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>8757646754245</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="24">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="3">
         <v>32336</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>8757646754245</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="25">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3">
         <v>34717</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>9087654321234</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="3">
         <v>36891</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5678908765432</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="25">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3">
         <v>29519</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2134765432123</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="25">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="3">
         <v>37295</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4567895643214</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="25">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="3">
         <v>34839</v>
       </c>
     </row>
@@ -770,12 +1128,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,19 +1147,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,12 +1219,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,22 +1238,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -906,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D2" s="12">
         <v>2</v>
@@ -927,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D3" s="12">
         <v>5</v>
@@ -948,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
@@ -969,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5" s="16">
         <v>2</v>
@@ -990,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D6" s="16">
         <v>2</v>
@@ -1011,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D7" s="16">
         <v>3</v>
@@ -1032,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
@@ -1053,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D9" s="20">
         <v>2</v>
@@ -1074,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
@@ -1101,9 +1459,318 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>14.5</v>
+      </c>
+      <c r="E2">
+        <v>12000</v>
+      </c>
+      <c r="F2">
+        <v>2345675</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3">
+        <v>3.25</v>
+      </c>
+      <c r="E3">
+        <v>1200</v>
+      </c>
+      <c r="F3">
+        <v>2345675</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>0.15</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>30000</v>
+      </c>
+      <c r="F4">
+        <v>4561232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>346</v>
+      </c>
+      <c r="F5">
+        <v>7658732</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>19.78</v>
+      </c>
+      <c r="E6">
+        <v>99</v>
+      </c>
+      <c r="F6">
+        <v>123754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>0.65</v>
+      </c>
+      <c r="D7">
+        <v>1.25</v>
+      </c>
+      <c r="E7">
+        <v>4500</v>
+      </c>
+      <c r="F7">
+        <v>8790879</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <f>E2*D2</f>
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>600</v>
+      </c>
+      <c r="E3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="0">E3*D3</f>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>0.65</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1111,262 +1778,239 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>83</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>28</v>
+        <v>85</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2">
-        <v>14.5</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2345675</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44242</v>
       </c>
       <c r="D2">
-        <v>12000</v>
+        <v>14320</v>
       </c>
       <c r="E2">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>2345675</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3">
-        <v>3.25</v>
+      <c r="C3" s="3">
+        <v>44790</v>
       </c>
       <c r="D3">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="E3">
-        <v>2345675</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4561232</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44914</v>
       </c>
       <c r="D4">
-        <v>30000</v>
+        <v>41250</v>
       </c>
       <c r="E4">
-        <v>4561232</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5">
-        <v>25</v>
-      </c>
-      <c r="D5">
-        <v>346</v>
-      </c>
-      <c r="E5">
-        <v>7658732</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>19.78</v>
-      </c>
-      <c r="D6">
-        <v>99</v>
-      </c>
-      <c r="E6">
-        <v>123754</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7">
-        <v>1.25</v>
-      </c>
-      <c r="D7">
-        <v>4500</v>
-      </c>
-      <c r="E7">
-        <v>8790879</v>
-      </c>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2345675</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
+      <c r="B2">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2">
         <v>23579757</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7658732</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
         <v>63768753</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9876543</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
+      <c r="B4">
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4">
         <v>65986475</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2940510</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5">
         <v>24656853</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8790879</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
+      <c r="B6">
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6">
         <v>36864279</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4561232</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
+      <c r="B7">
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7">
         <v>97808969</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>123754</v>
       </c>
-      <c r="B8" t="s">
-        <v>38</v>
+      <c r="B8">
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8">
         <v>78047624</v>
       </c>
     </row>

</xml_diff>